<commit_message>
"Updated ExportController.php to modify column assignments and added conditional logic for PW26 and PW27. Also updated Template Progres Isian.xlsx."
</commit_message>
<xml_diff>
--- a/public/Template Otsus/Template Progres Isian.xlsx
+++ b/public/Template Otsus/Template Progres Isian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/Laravel Project/SiAPP Transda v2/public/Template Otsus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878BF48E-68E3-5141-86DB-2F0337CE0B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EA675C-7ED4-E94A-BD64-BFE5B8B4814D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="16780" xr2:uid="{65C6CBC2-1CF4-BC4D-A56C-76649E3F5809}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>PROGRES ISIAN SIAPP TRANSDA</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>: .............................................</t>
+  </si>
+  <si>
+    <t>NAMA PEMDA</t>
   </si>
 </sst>
 </file>
@@ -224,7 +227,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -578,10 +601,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:R28"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,22 +612,23 @@
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="42.5" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" customWidth="1"/>
-    <col min="5" max="18" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
+    <col min="6" max="19" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="27" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:18" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:19" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -612,9 +636,10 @@
       <c r="C4" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:19" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
@@ -625,19 +650,21 @@
         <v>4</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="8"/>
+      <c r="K6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -645,65 +672,67 @@
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
-    </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -717,15 +746,16 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-    </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S8" s="4"/>
+    </row>
+    <row r="9" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -739,13 +769,14 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
-    </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S9" s="4"/>
+    </row>
+    <row r="10" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -759,13 +790,14 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
-    </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S10" s="4"/>
+    </row>
+    <row r="11" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -779,13 +811,14 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
-    </row>
-    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S11" s="4"/>
+    </row>
+    <row r="12" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -799,13 +832,14 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
-    </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S12" s="4"/>
+    </row>
+    <row r="13" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -819,13 +853,14 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
-    </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S13" s="4"/>
+    </row>
+    <row r="14" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -839,13 +874,14 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
-    </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S14" s="4"/>
+    </row>
+    <row r="15" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -859,13 +895,14 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-    </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S15" s="4"/>
+    </row>
+    <row r="16" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -879,13 +916,14 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
-    </row>
-    <row r="17" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -899,13 +937,14 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
-    </row>
-    <row r="18" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S17" s="4"/>
+    </row>
+    <row r="18" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -919,13 +958,14 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
-    </row>
-    <row r="19" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S18" s="4"/>
+    </row>
+    <row r="19" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -939,13 +979,14 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-    </row>
-    <row r="20" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S19" s="4"/>
+    </row>
+    <row r="20" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -959,13 +1000,14 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-    </row>
-    <row r="21" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S20" s="4"/>
+    </row>
+    <row r="21" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -979,13 +1021,14 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
-    </row>
-    <row r="22" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S21" s="4"/>
+    </row>
+    <row r="22" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -999,13 +1042,14 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
-    </row>
-    <row r="23" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S22" s="4"/>
+    </row>
+    <row r="23" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1019,13 +1063,14 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
-    </row>
-    <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S23" s="4"/>
+    </row>
+    <row r="24" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1039,13 +1084,14 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
-    </row>
-    <row r="25" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S24" s="4"/>
+    </row>
+    <row r="25" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1059,13 +1105,14 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
-    </row>
-    <row r="26" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S25" s="4"/>
+    </row>
+    <row r="26" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1079,13 +1126,14 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
-    </row>
-    <row r="27" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S26" s="4"/>
+    </row>
+    <row r="27" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1099,13 +1147,14 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
-    </row>
-    <row r="28" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S27" s="4"/>
+    </row>
+    <row r="28" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -1119,22 +1168,179 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+    </row>
+    <row r="29" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+    </row>
+    <row r="30" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+    </row>
+    <row r="31" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+    </row>
+    <row r="32" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+    </row>
+    <row r="33" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+    </row>
+    <row r="34" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+    </row>
+    <row r="35" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="J6:R6"/>
+  <mergeCells count="7">
+    <mergeCell ref="K6:S6"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="D6:D7"/>
   </mergeCells>
-  <conditionalFormatting sqref="E8:R28">
+  <conditionalFormatting sqref="F8:S28">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="SUDAH">
+      <formula>NOT(ISERROR(SEARCH("SUDAH",F8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="BELUM">
+      <formula>NOT(ISERROR(SEARCH("BELUM",F8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29:S35">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="SUDAH">
-      <formula>NOT(ISERROR(SEARCH("SUDAH",E8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("SUDAH",F29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="BELUM">
-      <formula>NOT(ISERROR(SEARCH("BELUM",E8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("BELUM",F29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>